<commit_message>
Computed Depression outcomes, also found error in depression/eating outcomes (corrected)
</commit_message>
<xml_diff>
--- a/larson(eating_es_ma).xlsx
+++ b/larson(eating_es_ma).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\Thesis\githubthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645C9D3E-8658-4C01-9CDA-753A21E4DCF8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFECDBD-37A3-4E0C-B22C-910B4354B7D6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11475" xr2:uid="{82994317-DEF0-47CC-A78E-074601CFA1DC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="35">
   <si>
     <t>eating</t>
   </si>
@@ -124,13 +124,19 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Emotional Eating Scale-Depression</t>
+  </si>
+  <si>
+    <t>Emotional Eating Scale-Anxiety</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +152,11 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -170,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -179,6 +190,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -497,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C3EF8B-CDE0-4990-9AD7-9A3620019349}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,27 +1520,85 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2010</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32">
+        <v>43</v>
+      </c>
+      <c r="G32" s="1">
+        <v>43</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>15</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2010</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33">
+        <v>43</v>
+      </c>
+      <c r="G33">
+        <v>43</v>
+      </c>
+      <c r="H33" s="1">
+        <v>-0.34</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E39" s="1"/>
     </row>
     <row r="74" spans="11:11" x14ac:dyDescent="0.25">

</xml_diff>